<commit_message>
Alles fresh inkl Geopandas
</commit_message>
<xml_diff>
--- a/12 Pandas Teil 4/dataprojects/Worldbank/formatted_table.xlsx
+++ b/12 Pandas Teil 4/dataprojects/Worldbank/formatted_table.xlsx
@@ -912,50 +912,50 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="106" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="106" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="107" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="108" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="109" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="110" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="110" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="111" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="112" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="113" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="113" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="114" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="114" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="115" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="115" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="15" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="116" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="16" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="18" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="19" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="117" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="20" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="21" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="118" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="118" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="22" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="119" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="119" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="24" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="25" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="26" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="120" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="120" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="27" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="28" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="30" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="31" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="121" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -963,13 +963,13 @@
     <xf numFmtId="0" fontId="3" fillId="122" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="33" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="34" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="123" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="123" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="35" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="36" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="124" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="37" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="38" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="125" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="125" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="39" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="40" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="41" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -977,7 +977,7 @@
     <xf numFmtId="0" fontId="3" fillId="42" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="127" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="43" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="128" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="128" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="44" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="45" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="46" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -985,60 +985,60 @@
     <xf numFmtId="0" fontId="2" fillId="47" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="130" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="48" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="131" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="131" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="49" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="50" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="132" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="51" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="133" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="52" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="52" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="134" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="53" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="135" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="135" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="54" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="136" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="137" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="137" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="55" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="138" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="139" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="139" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="56" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="140" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="141" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="140" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="141" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="57" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="58" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="59" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="60" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="60" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="61" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="142" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="143" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="62" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="62" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="144" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="145" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="63" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="146" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="146" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="64" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="65" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="66" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="147" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="148" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="149" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="66" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="147" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="148" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="149" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="67" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="150" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="68" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="69" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="69" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="151" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="70" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="152" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="71" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="72" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="73" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="74" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="72" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="73" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="74" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="75" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="153" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="154" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="154" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="76" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="77" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="155" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="155" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="156" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="78" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="79" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -1046,26 +1046,26 @@
     <xf numFmtId="0" fontId="2" fillId="158" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="80" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="81" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="159" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="159" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="82" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="160" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="83" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="84" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="85" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="161" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="86" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="162" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="86" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="162" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="87" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="163" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="88" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="163" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="88" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="164" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="89" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="90" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="165" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="91" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="91" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="166" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="92" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="93" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="93" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="167" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="94" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="95" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -1076,12 +1076,12 @@
     <xf numFmtId="0" fontId="2" fillId="169" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="99" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="100" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="101" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="101" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="102" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="103" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="104" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="170" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="105" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="170" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="105" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -4311,7 +4311,7 @@
       </c>
     </row>
     <row r="64">
-      <c r="A64" t="inlineStr">
+      <c r="A64" s="4" t="inlineStr">
         <is>
           <t>Algeria</t>
         </is>
@@ -6386,7 +6386,7 @@
           <t>Angola</t>
         </is>
       </c>
-      <c r="B110" t="inlineStr">
+      <c r="B110" s="4" t="inlineStr">
         <is>
           <t>AGO</t>
         </is>
@@ -6471,12 +6471,12 @@
       </c>
     </row>
     <row r="112">
-      <c r="A112" t="inlineStr">
+      <c r="A112" s="4" t="inlineStr">
         <is>
           <t>Zimbabwe</t>
         </is>
       </c>
-      <c r="B112" t="inlineStr">
+      <c r="B112" s="4" t="inlineStr">
         <is>
           <t>ZWE</t>
         </is>

</xml_diff>